<commit_message>
added vhost steps and validate address
</commit_message>
<xml_diff>
--- a/virtualShowData.xlsx
+++ b/virtualShowData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Katalon Studio\ShowMicrositeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>username</t>
   </si>
@@ -74,12 +74,6 @@
     <t>virtual_cabitest19</t>
   </si>
   <si>
-    <t>https://test3.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>cabitest3</t>
-  </si>
-  <si>
     <t>neoguest1 abc</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>ofbizPass</t>
   </si>
   <si>
-    <t>*******</t>
-  </si>
-  <si>
     <t>stylist</t>
   </si>
   <si>
@@ -131,9 +122,6 @@
     <t>verifyGuestCount</t>
   </si>
   <si>
-    <t>https://mirandakate.cabitest3.com/show-microsite/104515146/</t>
-  </si>
-  <si>
     <t>hostessMail</t>
   </si>
   <si>
@@ -167,25 +155,22 @@
     <t>guest2Mail</t>
   </si>
   <si>
+    <t>https://test19.cliotest.com/backoffice/control/main</t>
+  </si>
+  <si>
+    <t>C@bi$ush5</t>
+  </si>
+  <si>
+    <t>cabitest5</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>https://mirandakate.cabitest3.com/show-microsite/104515470/</t>
-  </si>
-  <si>
-    <t>https://mirandakate.cabitest3.com/show-microsite/104515472/</t>
-  </si>
-  <si>
-    <t>https://mirandakate.cabitest3.com/show-microsite/104515476/</t>
-  </si>
-  <si>
-    <t>https://mirandakate.cabitest3.com/show-microsite/104515478/</t>
-  </si>
-  <si>
-    <t>https://mirandakate.cabitest3.com/show-microsite/104515480/</t>
-  </si>
-  <si>
-    <t>https://mirandakate.cabitest3.com/show-microsite/104515482/</t>
+    <t>https://mirandakate.cabitest5.com/show-microsite/104516892/</t>
+  </si>
+  <si>
+    <t>https://mirandakate.cabitest5.com/show-microsite/104516894/</t>
   </si>
 </sst>
 </file>
@@ -521,13 +506,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="14.7109375" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="17.85546875" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
@@ -571,46 +556,46 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" t="s">
         <v>38</v>
       </c>
-      <c r="N1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" t="s">
-        <v>42</v>
-      </c>
       <c r="Q1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="S1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="T1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="U1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="V1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -627,74 +612,74 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="Q2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="S2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="T2">
         <v>2</v>
       </c>
       <c r="U2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="V2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -708,7 +693,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -717,12 +702,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A6" r:id="rId3"/>
-    <hyperlink ref="C6" r:id="rId4" display="C@bi$ush5"/>
-    <hyperlink ref="O2" r:id="rId5"/>
+    <hyperlink ref="A6" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="O2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed pushofbiz credentials from excel data file
</commit_message>
<xml_diff>
--- a/virtualShowData.xlsx
+++ b/virtualShowData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Katalon Studio\ShowMicrositeTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\katalon\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>username</t>
   </si>
@@ -65,9 +65,6 @@
     <t>https://pushofbiz.cliotest.com/login.php</t>
   </si>
   <si>
-    <t>sshinde</t>
-  </si>
-  <si>
     <t>vhostTarget</t>
   </si>
   <si>
@@ -155,22 +152,28 @@
     <t>guest2Mail</t>
   </si>
   <si>
-    <t>https://test19.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>C@bi$ush5</t>
-  </si>
-  <si>
-    <t>cabitest5</t>
+    <t>https://mirandakate.cabitest5.com/show-microsite/104516894/</t>
+  </si>
+  <si>
+    <t>https://test3.cliotest.com/backoffice/control/main</t>
+  </si>
+  <si>
+    <t>cabitest3</t>
+  </si>
+  <si>
+    <t>******</t>
+  </si>
+  <si>
+    <t>abcd</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>https://mirandakate.cabitest5.com/show-microsite/104516892/</t>
-  </si>
-  <si>
-    <t>https://mirandakate.cabitest5.com/show-microsite/104516894/</t>
+    <t>https://mirandakate.cabitest3.com/show-microsite/104526590/</t>
+  </si>
+  <si>
+    <t>https://mirandakate.cabitest3.com/show-microsite/104526592/</t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,7 @@
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,46 +559,46 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>36</v>
       </c>
-      <c r="M1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" t="s">
-        <v>38</v>
-      </c>
       <c r="Q1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -612,7 +615,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -621,68 +624,68 @@
         <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="Q2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T2">
         <v>2</v>
       </c>
       <c r="U2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -690,20 +693,20 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
     <hyperlink ref="A6" r:id="rId2"/>
-    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId3" display="C@bi$ush5"/>
     <hyperlink ref="O2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated url in xlsx
</commit_message>
<xml_diff>
--- a/virtualShowData.xlsx
+++ b/virtualShowData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\katalon\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>username</t>
   </si>
@@ -152,9 +152,6 @@
     <t>guest2Mail</t>
   </si>
   <si>
-    <t>https://mirandakate.cabitest5.com/show-microsite/104516894/</t>
-  </si>
-  <si>
     <t>https://test3.cliotest.com/backoffice/control/main</t>
   </si>
   <si>
@@ -167,21 +164,14 @@
     <t>abcd</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>https://mirandakate.cabitest3.com/show-microsite/104526590/</t>
-  </si>
-  <si>
-    <t>https://mirandakate.cabitest3.com/show-microsite/104526592/</t>
+    <t>https://mirandakate.cabitest4.com/show-microsite/104526592/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,27 +500,27 @@
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="48.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="10" max="16" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="48.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25" customWidth="1" collapsed="1"/>
+    <col min="10" max="16" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="22" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -621,10 +611,10 @@
         <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
         <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
       </c>
       <c r="I2" t="s">
         <v>38</v>
@@ -669,9 +659,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>49</v>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -693,10 +683,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -708,8 +698,9 @@
     <hyperlink ref="A6" r:id="rId2"/>
     <hyperlink ref="C6" r:id="rId3" display="C@bi$ush5"/>
     <hyperlink ref="O2" r:id="rId4"/>
+    <hyperlink ref="A3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
variable binding with two different excel files for two different test cases
</commit_message>
<xml_diff>
--- a/virtualShowData.xlsx
+++ b/virtualShowData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\katalon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\microsite_VS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>username</t>
   </si>
@@ -59,33 +59,9 @@
     <t>testEnvt</t>
   </si>
   <si>
-    <t>cabitTestEnvt</t>
-  </si>
-  <si>
-    <t>https://pushofbiz.cliotest.com/login.php</t>
-  </si>
-  <si>
-    <t>vhostTarget</t>
-  </si>
-  <si>
-    <t>virtual_cabitest19</t>
-  </si>
-  <si>
     <t>neoguest1 abc</t>
   </si>
   <si>
-    <t>neoguest1ab@test.com</t>
-  </si>
-  <si>
-    <t>ofbizURL</t>
-  </si>
-  <si>
-    <t>ofbizUser</t>
-  </si>
-  <si>
-    <t>ofbizPass</t>
-  </si>
-  <si>
     <t>stylist</t>
   </si>
   <si>
@@ -119,52 +95,13 @@
     <t>verifyGuestCount</t>
   </si>
   <si>
-    <t>hostessMail</t>
-  </si>
-  <si>
-    <t>cohostessMail</t>
-  </si>
-  <si>
-    <t>guest1Mail</t>
-  </si>
-  <si>
-    <t>hostessPass</t>
-  </si>
-  <si>
-    <t>cohostessPass</t>
-  </si>
-  <si>
-    <t>guest1Pass</t>
-  </si>
-  <si>
-    <t>guest2Pass</t>
-  </si>
-  <si>
-    <t>neohost1a@test.com</t>
-  </si>
-  <si>
-    <t>neocohost1a@test.com</t>
-  </si>
-  <si>
-    <t>neoguest2ab@test.com</t>
-  </si>
-  <si>
-    <t>guest2Mail</t>
-  </si>
-  <si>
-    <t>https://test3.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>cabitest3</t>
-  </si>
-  <si>
-    <t>******</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>https://mirandakate.cabitest4.com/show-microsite/104526592/</t>
+    <t>cabiTestEnvt</t>
+  </si>
+  <si>
+    <t>https://test19.cliotest.com/backoffice/control/main</t>
+  </si>
+  <si>
+    <t>cabitest5</t>
   </si>
 </sst>
 </file>
@@ -497,24 +434,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="44.140625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="48.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="25" customWidth="1" collapsed="1"/>
-    <col min="10" max="16" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="13.85546875" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="22" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="23.5703125" customWidth="1" collapsed="1"/>
@@ -523,184 +464,99 @@
     <col min="22" max="22" width="19.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1">
+        <v>400000002</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>400000002</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>2</v>
+      <c r="L2" t="s">
+        <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
         <v>25</v>
-      </c>
-      <c r="T2">
-        <v>2</v>
-      </c>
-      <c r="U2" t="s">
-        <v>29</v>
-      </c>
-      <c r="V2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="A6" r:id="rId2"/>
-    <hyperlink ref="C6" r:id="rId3" display="C@bi$ush5"/>
-    <hyperlink ref="O2" r:id="rId4"/>
-    <hyperlink ref="A3" r:id="rId5"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>